<commit_message>
add excel for html code
</commit_message>
<xml_diff>
--- a/html_versions_for_loopMerge.xlsx
+++ b/html_versions_for_loopMerge.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="6810"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="6810" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet18" sheetId="52" r:id="rId1"/>
     <sheet name="Sheet20" sheetId="54" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="55" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="56" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="291">
   <si>
     <t>&lt;style&gt;body{background-image:url('https://raw.githubusercontent.com/pb6191/mockBankingImages/master/white-paper-texture-1152962.jpg');}&lt;/style&gt;</t>
   </si>
@@ -344,19 +346,608 @@
   <si>
     <t xml:space="preserve">&lt;style&gt;body{background-image:url('https://raw.githubusercontent.com/pb6191/mockBankingImages/master/white-paper-texture-1152962.jpg');}&lt;/style&gt;&lt;h1&gt;&lt;span style="font-weight: 400;"&gt;Connor Wood&lt;/span&gt;&lt;/h1&gt;&lt;p&gt;&lt;strong&gt;Personal Details&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;Gender:&amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &lt;/span&gt; &lt;span style="font-weight: 400;"&gt;&amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &lt;/span&gt; &lt;span style="font-weight: 400;"&gt;Male&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;Date of Birth: &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &lt;/span&gt; &lt;span style="font-weight: 400;"&gt;11/10/1997&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Education&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;2015-2019&amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &lt;/span&gt; &lt;strong&gt;Michigan State University&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/span&gt; &lt;span style="font-weight: 400;"&gt;East Lansing, Michigan&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;&lt;span style="font-weight: 400;"&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/span&gt;Bachelor&amp;rsquo;s of Arts&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Work Experience&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;2019-present &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &lt;/span&gt; &lt;strong&gt;Human Resource Manager&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="font-weight: 400;"&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/span&gt; &lt;strong&gt;City of Detroit - Detroit, MI&lt;/strong&gt;&lt;/p&gt;&lt;ol&gt;&lt;li style="font-weight: 400;"&gt;&lt;span style="font-weight: 400;"&gt;A HR Director overseeing the management and direction of the Recruitment and Selection Division of Local Government - A Division of high volume staffing and recruitment activities for the entire municipality.&lt;/span&gt;&lt;/li&gt;&lt;li style="font-weight: 400;"&gt;&lt;span style="font-weight: 400;"&gt;Governed a $1.5 million budget&lt;/span&gt;&lt;/li&gt;&lt;li style="font-weight: 400;"&gt;&lt;span style="font-weight: 400;"&gt;Managed 40 direct reports in the following five subdivisions: Recruitment, Job Employment Center, Testing, Workforce Planning and Affirmative Action.&lt;/span&gt;&lt;/li&gt;&lt;li style="font-weight: 400;"&gt;&lt;span style="font-weight: 400;"&gt;Managed the talent acquisition process (including consulting with HR and other business partners to identify staffing needs, design and implement attraction strategies, ensuring clear job skill specifications, internal and external sourcing, candidate screening, and facilitation of background checks and offer consultation, immigration and hiring processes).&lt;/span&gt;&lt;/li&gt;&lt;li style="font-weight: 400;"&gt;&lt;span style="font-weight: 400;"&gt;Assisted in driving the strategic programs, policies, platforms, services and tools that enable the City to align staffing with the workforce plans. Developed and managed relationships with staffing vendor organizations and educational institutions.&lt;/span&gt;&lt;/li&gt;&lt;/ol&gt;
 </t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1</t>
+  </si>
+  <si>
+    <t>.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1</t>
+  </si>
+  <si>
+    <t>.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24.png</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24</t>
+  </si>
+  <si>
+    <t>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;a data-lightbox="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24.png" data-title="" href="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24.png"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24.png" style="width:30%;"&gt;&lt;/a&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -376,16 +967,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -689,7 +1286,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1528,4 +2125,1392 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE(A1, B1)</f>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1.png</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" t="str">
+        <f>CONCATENATE(K1, L1)</f>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C24" si="0">CONCATENATE(A2, B2)</f>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2.png</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M24" si="1">CONCATENATE(K2, L2)</f>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_2.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3.png</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_3.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4.png</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_4.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5.png</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_5.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6.png</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_6.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7.png</v>
+      </c>
+      <c r="E7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K7" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_7.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8.png</v>
+      </c>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K8" t="s">
+        <v>129</v>
+      </c>
+      <c r="L8" t="s">
+        <v>101</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_8.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9.png</v>
+      </c>
+      <c r="E9" t="s">
+        <v>132</v>
+      </c>
+      <c r="K9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" t="s">
+        <v>101</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_9.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10.png</v>
+      </c>
+      <c r="E10" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" t="s">
+        <v>137</v>
+      </c>
+      <c r="L10" t="s">
+        <v>101</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_10.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11.png</v>
+      </c>
+      <c r="E11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L11" t="s">
+        <v>101</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_11.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12.png</v>
+      </c>
+      <c r="E12" t="s">
+        <v>144</v>
+      </c>
+      <c r="K12" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_12.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13.png</v>
+      </c>
+      <c r="E13" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" t="s">
+        <v>149</v>
+      </c>
+      <c r="L13" t="s">
+        <v>101</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_13.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14.png</v>
+      </c>
+      <c r="E14" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" t="s">
+        <v>153</v>
+      </c>
+      <c r="L14" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_14.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15.png</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+      <c r="K15" t="s">
+        <v>157</v>
+      </c>
+      <c r="L15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_15.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16.png</v>
+      </c>
+      <c r="E16" t="s">
+        <v>160</v>
+      </c>
+      <c r="K16" t="s">
+        <v>161</v>
+      </c>
+      <c r="L16" t="s">
+        <v>101</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_16.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17.png</v>
+      </c>
+      <c r="E17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K17" t="s">
+        <v>165</v>
+      </c>
+      <c r="L17" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_17.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18.png</v>
+      </c>
+      <c r="E18" t="s">
+        <v>168</v>
+      </c>
+      <c r="K18" t="s">
+        <v>169</v>
+      </c>
+      <c r="L18" t="s">
+        <v>101</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_18.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19.png</v>
+      </c>
+      <c r="E19" t="s">
+        <v>172</v>
+      </c>
+      <c r="K19" t="s">
+        <v>173</v>
+      </c>
+      <c r="L19" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_19.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20.png</v>
+      </c>
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+      <c r="K20" t="s">
+        <v>177</v>
+      </c>
+      <c r="L20" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_20.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21.png</v>
+      </c>
+      <c r="E21" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" t="s">
+        <v>181</v>
+      </c>
+      <c r="L21" t="s">
+        <v>101</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_21.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22.png</v>
+      </c>
+      <c r="E22" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" t="s">
+        <v>185</v>
+      </c>
+      <c r="L22" t="s">
+        <v>101</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_22.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23.png</v>
+      </c>
+      <c r="E23" t="s">
+        <v>188</v>
+      </c>
+      <c r="K23" t="s">
+        <v>189</v>
+      </c>
+      <c r="L23" t="s">
+        <v>101</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_23.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24.png</v>
+      </c>
+      <c r="E24" t="s">
+        <v>192</v>
+      </c>
+      <c r="K24" t="s">
+        <v>193</v>
+      </c>
+      <c r="L24" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_24.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2:A8" r:id="rId2" display="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1"/>
+    <hyperlink ref="A9" r:id="rId3" display="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1"/>
+    <hyperlink ref="A17" r:id="rId4" display="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1"/>
+    <hyperlink ref="A10:A16" r:id="rId5" display="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1"/>
+    <hyperlink ref="A18:A24" r:id="rId6" display="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_banking/banking_1"/>
+    <hyperlink ref="E1" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE(A1, B1)</f>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1.png</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" t="str">
+        <f t="shared" ref="M1:M24" si="0">CONCATENATE(K1, L1)</f>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D24" si="1">CONCATENATE(A2, B2)</f>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2.png</v>
+      </c>
+      <c r="H2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K2" t="s">
+        <v>201</v>
+      </c>
+      <c r="L2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_2.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3.png</v>
+      </c>
+      <c r="H3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_3.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4.png</v>
+      </c>
+      <c r="H4" t="s">
+        <v>208</v>
+      </c>
+      <c r="K4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_4.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5.png</v>
+      </c>
+      <c r="H5" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" t="s">
+        <v>213</v>
+      </c>
+      <c r="L5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_5.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6.png</v>
+      </c>
+      <c r="H6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_6.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7.png</v>
+      </c>
+      <c r="H7" t="s">
+        <v>220</v>
+      </c>
+      <c r="K7" t="s">
+        <v>221</v>
+      </c>
+      <c r="L7" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_7.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8.png</v>
+      </c>
+      <c r="H8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K8" t="s">
+        <v>225</v>
+      </c>
+      <c r="L8" t="s">
+        <v>101</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_8.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9.png</v>
+      </c>
+      <c r="H9" t="s">
+        <v>228</v>
+      </c>
+      <c r="K9" t="s">
+        <v>229</v>
+      </c>
+      <c r="L9" t="s">
+        <v>101</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_9.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10.png</v>
+      </c>
+      <c r="H10" t="s">
+        <v>232</v>
+      </c>
+      <c r="K10" t="s">
+        <v>233</v>
+      </c>
+      <c r="L10" t="s">
+        <v>101</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_10.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11.png</v>
+      </c>
+      <c r="H11" t="s">
+        <v>236</v>
+      </c>
+      <c r="K11" t="s">
+        <v>237</v>
+      </c>
+      <c r="L11" t="s">
+        <v>101</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_11.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12.png</v>
+      </c>
+      <c r="H12" t="s">
+        <v>240</v>
+      </c>
+      <c r="K12" t="s">
+        <v>241</v>
+      </c>
+      <c r="L12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_12.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13.png</v>
+      </c>
+      <c r="H13" t="s">
+        <v>244</v>
+      </c>
+      <c r="K13" t="s">
+        <v>245</v>
+      </c>
+      <c r="L13" t="s">
+        <v>101</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_13.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14.png</v>
+      </c>
+      <c r="H14" t="s">
+        <v>248</v>
+      </c>
+      <c r="K14" t="s">
+        <v>249</v>
+      </c>
+      <c r="L14" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_14.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15.png</v>
+      </c>
+      <c r="H15" t="s">
+        <v>252</v>
+      </c>
+      <c r="K15" t="s">
+        <v>253</v>
+      </c>
+      <c r="L15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_15.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16.png</v>
+      </c>
+      <c r="H16" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" t="s">
+        <v>257</v>
+      </c>
+      <c r="L16" t="s">
+        <v>101</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_16.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17.png</v>
+      </c>
+      <c r="H17" t="s">
+        <v>260</v>
+      </c>
+      <c r="K17" t="s">
+        <v>261</v>
+      </c>
+      <c r="L17" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_17.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18.png</v>
+      </c>
+      <c r="H18" t="s">
+        <v>264</v>
+      </c>
+      <c r="K18" t="s">
+        <v>265</v>
+      </c>
+      <c r="L18" t="s">
+        <v>101</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_18.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19.png</v>
+      </c>
+      <c r="H19" t="s">
+        <v>268</v>
+      </c>
+      <c r="K19" t="s">
+        <v>269</v>
+      </c>
+      <c r="L19" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_19.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20.png</v>
+      </c>
+      <c r="H20" t="s">
+        <v>272</v>
+      </c>
+      <c r="K20" t="s">
+        <v>273</v>
+      </c>
+      <c r="L20" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_20.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21.png</v>
+      </c>
+      <c r="H21" t="s">
+        <v>276</v>
+      </c>
+      <c r="K21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L21" t="s">
+        <v>101</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_21.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22.png</v>
+      </c>
+      <c r="H22" t="s">
+        <v>280</v>
+      </c>
+      <c r="K22" t="s">
+        <v>281</v>
+      </c>
+      <c r="L22" t="s">
+        <v>101</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_22.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23.png</v>
+      </c>
+      <c r="H23" t="s">
+        <v>284</v>
+      </c>
+      <c r="K23" t="s">
+        <v>285</v>
+      </c>
+      <c r="L23" t="s">
+        <v>101</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_23.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24.png</v>
+      </c>
+      <c r="H24" t="s">
+        <v>288</v>
+      </c>
+      <c r="K24" t="s">
+        <v>289</v>
+      </c>
+      <c r="L24" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div style="text-align: left;"&gt;&lt;span style="font-family:Times New Roman,Times,serif;"&gt;&lt;span style="font-size:19px;"&gt;&lt;img src="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_24.png" style="width:30%;"&gt;&lt;/span&gt;&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="N24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2:A24" r:id="rId2" display="https://raw.githubusercontent.com/pb6191/mockBankingImages/master/resumes_hr/hr_1"/>
+    <hyperlink ref="H1" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>